<commit_message>
Actualizar el modelo de plano de empresa y la viabilidad inicial con nuevos datos financieros y ajustes en los costos.
</commit_message>
<xml_diff>
--- a/Viabilidade inicial Modelo.xlsx
+++ b/Viabilidade inicial Modelo.xlsx
@@ -23,6 +23,7 @@
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm.Print_Area" vbProcedure="false">CANVAS!$B$2:$G$34</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm.Print_Area" vbProcedure="false">CANVAS!$B$2:$G$34</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm.Print_Area_0" vbProcedure="false">CANVAS!$B$2:$G$34</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm.Print_Area_0_0" vbProcedure="false">CANVAS!$B$2:$G$34</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -2397,8 +2398,7 @@
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
     <cellStyle name="Excel Built-in Explanatory Text" xfId="37" builtinId="53" customBuiltin="true"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf/>
+  <dxfs count="3">
     <dxf/>
     <dxf/>
     <dxf/>
@@ -2473,7 +2473,7 @@
   </sheetPr>
   <dimension ref="B1:U13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -2589,7 +2589,7 @@
   </sheetPr>
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -2796,7 +2796,7 @@
   </sheetPr>
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -2849,7 +2849,7 @@
   </sheetPr>
   <dimension ref="A1:V23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -3139,7 +3139,7 @@
   </sheetPr>
   <dimension ref="A1:S33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
@@ -3883,7 +3883,7 @@
   </sheetPr>
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -4333,7 +4333,7 @@
   </sheetPr>
   <dimension ref="A1:K45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B32" activeCellId="0" sqref="B32"/>
     </sheetView>
   </sheetViews>
@@ -5067,7 +5067,7 @@
   </sheetPr>
   <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
     </sheetView>
   </sheetViews>
@@ -5794,8 +5794,8 @@
   </sheetPr>
   <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E20" activeCellId="0" sqref="E20"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G26" activeCellId="0" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6266,13 +6266,14 @@
     </row>
   </sheetData>
   <sheetProtection sheet="true" password="946e" objects="true" scenarios="true"/>
-  <mergeCells count="7">
+  <mergeCells count="8">
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="C16:C17"/>
+    <mergeCell ref="C19:C20"/>
     <mergeCell ref="C32:C33"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -6292,7 +6293,7 @@
   </sheetPr>
   <dimension ref="B2:G35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J11" activeCellId="0" sqref="J11"/>
     </sheetView>
   </sheetViews>

</xml_diff>